<commit_message>
update comment in excel file
</commit_message>
<xml_diff>
--- a/storage/app/Agroecology Funding Tool - Initiative Import Template.xlsx
+++ b/storage/app/Agroecology Funding Tool - Initiative Import Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanTang\Documents\01. Projects\12. AEC\20230713 Import Excel File Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/aec_portfolio/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDFCA22-B04D-4C92-8F05-A78466CEEFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1935734A-AF35-C546-80AD-C304824A360A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21569DC4-0C9C-9A4F-A7E1-7EA7911B1920}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{21569DC4-0C9C-9A4F-A7E1-7EA7911B1920}"/>
   </bookViews>
   <sheets>
     <sheet name="projects" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>exchange_rate</t>
   </si>
   <si>
-    <t>1 of this initiative's currency = XXX EUR</t>
-  </si>
-  <si>
     <t>the institution or entity that directly receives the majority of the funds for this initiative</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>main_recipient</t>
+  </si>
+  <si>
+    <t>1 of this initiative's currency = XXX of your organisation's default currency.</t>
   </si>
 </sst>
 </file>
@@ -540,25 +540,25 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.375" customWidth="1"/>
-    <col min="3" max="3" width="42.375" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="14.625" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="11" max="11" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="16.625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -578,10 +578,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -595,7 +595,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -609,16 +609,16 @@
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>18</v>
@@ -631,7 +631,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -651,10 +651,10 @@
         <v>500000</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="7">
         <v>44896</v>
@@ -666,7 +666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -677,2994 +677,2994 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G5" s="6"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G99" s="6"/>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G100" s="6"/>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G101" s="6"/>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G102" s="6"/>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G104" s="6"/>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G105" s="6"/>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G106" s="6"/>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G107" s="6"/>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G108" s="6"/>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G109" s="6"/>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G110" s="6"/>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G111" s="6"/>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G112" s="6"/>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G113" s="6"/>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G114" s="6"/>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G115" s="6"/>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G116" s="6"/>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G117" s="6"/>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G118" s="6"/>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G119" s="6"/>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G120" s="6"/>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G121" s="6"/>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G122" s="6"/>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G123" s="6"/>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G124" s="6"/>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G125" s="6"/>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G126" s="6"/>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G127" s="6"/>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G128" s="6"/>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G129" s="6"/>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G130" s="6"/>
     </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G131" s="6"/>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G132" s="6"/>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G133" s="6"/>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G134" s="6"/>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G135" s="6"/>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G136" s="6"/>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G137" s="6"/>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G138" s="6"/>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G139" s="6"/>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G140" s="6"/>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G141" s="6"/>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G142" s="6"/>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G143" s="6"/>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G144" s="6"/>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G145" s="6"/>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G146" s="6"/>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G147" s="6"/>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G148" s="6"/>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G149" s="6"/>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G150" s="6"/>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G151" s="6"/>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G152" s="6"/>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G153" s="6"/>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G154" s="6"/>
     </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G155" s="6"/>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G156" s="6"/>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G157" s="6"/>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G158" s="6"/>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G159" s="6"/>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G160" s="6"/>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G161" s="6"/>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G162" s="6"/>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G163" s="6"/>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G164" s="6"/>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G165" s="6"/>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G166" s="6"/>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G167" s="6"/>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G168" s="6"/>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G169" s="6"/>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G170" s="6"/>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G171" s="6"/>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G172" s="6"/>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G173" s="6"/>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G174" s="6"/>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G175" s="6"/>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G176" s="6"/>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G177" s="6"/>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G178" s="6"/>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G179" s="6"/>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G180" s="6"/>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G181" s="6"/>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G182" s="6"/>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G183" s="6"/>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G184" s="6"/>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G185" s="6"/>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G186" s="6"/>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G187" s="6"/>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G188" s="6"/>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G189" s="6"/>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G190" s="6"/>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G191" s="6"/>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G192" s="6"/>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G193" s="6"/>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G194" s="6"/>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G195" s="6"/>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G196" s="6"/>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G197" s="6"/>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G198" s="6"/>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G199" s="6"/>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G200" s="6"/>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G201" s="6"/>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G202" s="6"/>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G203" s="6"/>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G204" s="6"/>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G205" s="6"/>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G206" s="6"/>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G207" s="6"/>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G208" s="6"/>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G209" s="6"/>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G210" s="6"/>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G211" s="6"/>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G212" s="6"/>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G213" s="6"/>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G214" s="6"/>
     </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G215" s="6"/>
     </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G216" s="6"/>
     </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G217" s="6"/>
     </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G218" s="6"/>
     </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G219" s="6"/>
     </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G220" s="6"/>
     </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G221" s="6"/>
     </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G222" s="6"/>
     </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G223" s="6"/>
     </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G224" s="6"/>
     </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G225" s="6"/>
     </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G226" s="6"/>
     </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G227" s="6"/>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G228" s="6"/>
     </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G229" s="6"/>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G230" s="6"/>
     </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G231" s="6"/>
     </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G232" s="6"/>
     </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G233" s="6"/>
     </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G234" s="6"/>
     </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G235" s="6"/>
     </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G236" s="6"/>
     </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G237" s="6"/>
     </row>
-    <row r="238" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G238" s="6"/>
     </row>
-    <row r="239" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G239" s="6"/>
     </row>
-    <row r="240" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G240" s="6"/>
     </row>
-    <row r="241" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G241" s="6"/>
     </row>
-    <row r="242" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G242" s="6"/>
     </row>
-    <row r="243" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G243" s="6"/>
     </row>
-    <row r="244" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G244" s="6"/>
     </row>
-    <row r="245" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G245" s="6"/>
     </row>
-    <row r="246" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G246" s="6"/>
     </row>
-    <row r="247" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G247" s="6"/>
     </row>
-    <row r="248" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G248" s="6"/>
     </row>
-    <row r="249" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G249" s="6"/>
     </row>
-    <row r="250" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G250" s="6"/>
     </row>
-    <row r="251" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G251" s="6"/>
     </row>
-    <row r="252" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G252" s="6"/>
     </row>
-    <row r="253" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G253" s="6"/>
     </row>
-    <row r="254" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G254" s="6"/>
     </row>
-    <row r="255" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G255" s="6"/>
     </row>
-    <row r="256" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G256" s="6"/>
     </row>
-    <row r="257" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G257" s="6"/>
     </row>
-    <row r="258" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G258" s="6"/>
     </row>
-    <row r="259" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G259" s="6"/>
     </row>
-    <row r="260" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G260" s="6"/>
     </row>
-    <row r="261" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G261" s="6"/>
     </row>
-    <row r="262" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G262" s="6"/>
     </row>
-    <row r="263" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G263" s="6"/>
     </row>
-    <row r="264" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G264" s="6"/>
     </row>
-    <row r="265" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G265" s="6"/>
     </row>
-    <row r="266" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G266" s="6"/>
     </row>
-    <row r="267" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G267" s="6"/>
     </row>
-    <row r="268" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G268" s="6"/>
     </row>
-    <row r="269" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G269" s="6"/>
     </row>
-    <row r="270" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G270" s="6"/>
     </row>
-    <row r="271" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G271" s="6"/>
     </row>
-    <row r="272" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G272" s="6"/>
     </row>
-    <row r="273" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G273" s="6"/>
     </row>
-    <row r="274" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G274" s="6"/>
     </row>
-    <row r="275" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G275" s="6"/>
     </row>
-    <row r="276" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G276" s="6"/>
     </row>
-    <row r="277" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G277" s="6"/>
     </row>
-    <row r="278" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G278" s="6"/>
     </row>
-    <row r="279" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G279" s="6"/>
     </row>
-    <row r="280" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G280" s="6"/>
     </row>
-    <row r="281" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G281" s="6"/>
     </row>
-    <row r="282" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G282" s="6"/>
     </row>
-    <row r="283" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G283" s="6"/>
     </row>
-    <row r="284" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G284" s="6"/>
     </row>
-    <row r="285" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G285" s="6"/>
     </row>
-    <row r="286" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G286" s="6"/>
     </row>
-    <row r="287" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G287" s="6"/>
     </row>
-    <row r="288" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G288" s="6"/>
     </row>
-    <row r="289" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G289" s="6"/>
     </row>
-    <row r="290" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G290" s="6"/>
     </row>
-    <row r="291" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G291" s="6"/>
     </row>
-    <row r="292" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G292" s="6"/>
     </row>
-    <row r="293" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G293" s="6"/>
     </row>
-    <row r="294" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G294" s="6"/>
     </row>
-    <row r="295" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G295" s="6"/>
     </row>
-    <row r="296" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G296" s="6"/>
     </row>
-    <row r="297" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G297" s="6"/>
     </row>
-    <row r="298" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G298" s="6"/>
     </row>
-    <row r="299" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G299" s="6"/>
     </row>
-    <row r="300" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G300" s="6"/>
     </row>
-    <row r="301" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G301" s="6"/>
     </row>
-    <row r="302" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="302" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G302" s="6"/>
     </row>
-    <row r="303" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="303" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G303" s="6"/>
     </row>
-    <row r="304" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="304" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G304" s="6"/>
     </row>
-    <row r="305" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G305" s="6"/>
     </row>
-    <row r="306" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="306" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G306" s="6"/>
     </row>
-    <row r="307" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G307" s="6"/>
     </row>
-    <row r="308" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="308" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G308" s="6"/>
     </row>
-    <row r="309" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G309" s="6"/>
     </row>
-    <row r="310" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G310" s="6"/>
     </row>
-    <row r="311" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G311" s="6"/>
     </row>
-    <row r="312" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G312" s="6"/>
     </row>
-    <row r="313" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="313" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G313" s="6"/>
     </row>
-    <row r="314" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G314" s="6"/>
     </row>
-    <row r="315" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G315" s="6"/>
     </row>
-    <row r="316" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G316" s="6"/>
     </row>
-    <row r="317" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G317" s="6"/>
     </row>
-    <row r="318" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="318" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G318" s="6"/>
     </row>
-    <row r="319" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G319" s="6"/>
     </row>
-    <row r="320" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G320" s="6"/>
     </row>
-    <row r="321" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="321" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G321" s="6"/>
     </row>
-    <row r="322" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="322" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G322" s="6"/>
     </row>
-    <row r="323" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="323" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G323" s="6"/>
     </row>
-    <row r="324" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="324" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G324" s="6"/>
     </row>
-    <row r="325" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="325" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G325" s="6"/>
     </row>
-    <row r="326" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="326" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G326" s="6"/>
     </row>
-    <row r="327" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="327" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G327" s="6"/>
     </row>
-    <row r="328" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="328" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G328" s="6"/>
     </row>
-    <row r="329" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="329" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G329" s="6"/>
     </row>
-    <row r="330" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="330" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G330" s="6"/>
     </row>
-    <row r="331" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="331" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G331" s="6"/>
     </row>
-    <row r="332" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="332" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G332" s="6"/>
     </row>
-    <row r="333" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="333" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G333" s="6"/>
     </row>
-    <row r="334" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="334" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G334" s="6"/>
     </row>
-    <row r="335" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="335" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G335" s="6"/>
     </row>
-    <row r="336" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="336" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G336" s="6"/>
     </row>
-    <row r="337" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="337" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G337" s="6"/>
     </row>
-    <row r="338" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="338" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G338" s="6"/>
     </row>
-    <row r="339" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="339" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G339" s="6"/>
     </row>
-    <row r="340" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="340" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G340" s="6"/>
     </row>
-    <row r="341" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="341" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G341" s="6"/>
     </row>
-    <row r="342" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="342" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G342" s="6"/>
     </row>
-    <row r="343" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="343" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G343" s="6"/>
     </row>
-    <row r="344" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="344" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G344" s="6"/>
     </row>
-    <row r="345" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="345" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G345" s="6"/>
     </row>
-    <row r="346" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="346" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G346" s="6"/>
     </row>
-    <row r="347" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="347" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G347" s="6"/>
     </row>
-    <row r="348" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="348" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G348" s="6"/>
     </row>
-    <row r="349" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="349" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G349" s="6"/>
     </row>
-    <row r="350" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="350" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G350" s="6"/>
     </row>
-    <row r="351" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="351" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G351" s="6"/>
     </row>
-    <row r="352" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="352" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G352" s="6"/>
     </row>
-    <row r="353" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="353" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G353" s="6"/>
     </row>
-    <row r="354" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="354" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G354" s="6"/>
     </row>
-    <row r="355" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="355" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G355" s="6"/>
     </row>
-    <row r="356" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="356" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G356" s="6"/>
     </row>
-    <row r="357" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="357" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G357" s="6"/>
     </row>
-    <row r="358" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="358" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G358" s="6"/>
     </row>
-    <row r="359" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="359" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G359" s="6"/>
     </row>
-    <row r="360" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="360" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G360" s="6"/>
     </row>
-    <row r="361" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="361" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G361" s="6"/>
     </row>
-    <row r="362" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="362" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G362" s="6"/>
     </row>
-    <row r="363" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="363" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G363" s="6"/>
     </row>
-    <row r="364" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="364" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G364" s="6"/>
     </row>
-    <row r="365" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="365" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G365" s="6"/>
     </row>
-    <row r="366" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="366" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G366" s="6"/>
     </row>
-    <row r="367" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="367" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G367" s="6"/>
     </row>
-    <row r="368" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="368" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G368" s="6"/>
     </row>
-    <row r="369" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G369" s="6"/>
     </row>
-    <row r="370" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="370" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G370" s="6"/>
     </row>
-    <row r="371" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="371" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G371" s="6"/>
     </row>
-    <row r="372" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="372" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G372" s="6"/>
     </row>
-    <row r="373" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="373" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G373" s="6"/>
     </row>
-    <row r="374" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="374" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G374" s="6"/>
     </row>
-    <row r="375" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="375" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G375" s="6"/>
     </row>
-    <row r="376" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="376" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G376" s="6"/>
     </row>
-    <row r="377" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="377" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G377" s="6"/>
     </row>
-    <row r="378" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="378" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G378" s="6"/>
     </row>
-    <row r="379" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="379" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G379" s="6"/>
     </row>
-    <row r="380" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="380" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G380" s="6"/>
     </row>
-    <row r="381" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="381" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G381" s="6"/>
     </row>
-    <row r="382" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="382" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G382" s="6"/>
     </row>
-    <row r="383" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="383" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G383" s="6"/>
     </row>
-    <row r="384" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="384" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G384" s="6"/>
     </row>
-    <row r="385" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="385" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G385" s="6"/>
     </row>
-    <row r="386" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="386" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G386" s="6"/>
     </row>
-    <row r="387" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="387" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G387" s="6"/>
     </row>
-    <row r="388" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="388" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G388" s="6"/>
     </row>
-    <row r="389" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="389" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G389" s="6"/>
     </row>
-    <row r="390" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="390" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G390" s="6"/>
     </row>
-    <row r="391" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="391" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G391" s="6"/>
     </row>
-    <row r="392" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="392" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G392" s="6"/>
     </row>
-    <row r="393" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="393" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G393" s="6"/>
     </row>
-    <row r="394" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="394" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G394" s="6"/>
     </row>
-    <row r="395" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="395" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G395" s="6"/>
     </row>
-    <row r="396" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="396" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G396" s="6"/>
     </row>
-    <row r="397" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="397" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G397" s="6"/>
     </row>
-    <row r="398" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="398" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G398" s="6"/>
     </row>
-    <row r="399" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="399" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G399" s="6"/>
     </row>
-    <row r="400" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="400" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G400" s="6"/>
     </row>
-    <row r="401" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="401" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G401" s="6"/>
     </row>
-    <row r="402" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="402" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G402" s="6"/>
     </row>
-    <row r="403" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="403" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G403" s="6"/>
     </row>
-    <row r="404" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="404" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G404" s="6"/>
     </row>
-    <row r="405" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="405" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G405" s="6"/>
     </row>
-    <row r="406" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="406" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G406" s="6"/>
     </row>
-    <row r="407" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="407" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G407" s="6"/>
     </row>
-    <row r="408" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="408" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G408" s="6"/>
     </row>
-    <row r="409" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="409" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G409" s="6"/>
     </row>
-    <row r="410" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="410" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G410" s="6"/>
     </row>
-    <row r="411" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="411" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G411" s="6"/>
     </row>
-    <row r="412" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="412" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G412" s="6"/>
     </row>
-    <row r="413" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="413" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G413" s="6"/>
     </row>
-    <row r="414" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="414" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G414" s="6"/>
     </row>
-    <row r="415" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="415" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G415" s="6"/>
     </row>
-    <row r="416" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="416" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G416" s="6"/>
     </row>
-    <row r="417" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="417" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G417" s="6"/>
     </row>
-    <row r="418" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="418" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G418" s="6"/>
     </row>
-    <row r="419" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="419" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G419" s="6"/>
     </row>
-    <row r="420" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="420" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G420" s="6"/>
     </row>
-    <row r="421" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="421" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G421" s="6"/>
     </row>
-    <row r="422" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="422" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G422" s="6"/>
     </row>
-    <row r="423" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="423" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G423" s="6"/>
     </row>
-    <row r="424" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="424" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G424" s="6"/>
     </row>
-    <row r="425" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="425" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G425" s="6"/>
     </row>
-    <row r="426" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="426" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G426" s="6"/>
     </row>
-    <row r="427" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="427" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G427" s="6"/>
     </row>
-    <row r="428" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="428" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G428" s="6"/>
     </row>
-    <row r="429" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="429" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G429" s="6"/>
     </row>
-    <row r="430" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="430" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G430" s="6"/>
     </row>
-    <row r="431" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="431" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G431" s="6"/>
     </row>
-    <row r="432" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="432" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G432" s="6"/>
     </row>
-    <row r="433" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="433" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G433" s="6"/>
     </row>
-    <row r="434" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="434" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G434" s="6"/>
     </row>
-    <row r="435" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="435" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G435" s="6"/>
     </row>
-    <row r="436" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="436" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G436" s="6"/>
     </row>
-    <row r="437" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="437" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G437" s="6"/>
     </row>
-    <row r="438" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="438" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G438" s="6"/>
     </row>
-    <row r="439" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="439" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G439" s="6"/>
     </row>
-    <row r="440" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="440" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G440" s="6"/>
     </row>
-    <row r="441" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="441" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G441" s="6"/>
     </row>
-    <row r="442" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="442" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G442" s="6"/>
     </row>
-    <row r="443" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="443" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G443" s="6"/>
     </row>
-    <row r="444" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="444" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G444" s="6"/>
     </row>
-    <row r="445" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="445" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G445" s="6"/>
     </row>
-    <row r="446" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="446" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G446" s="6"/>
     </row>
-    <row r="447" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="447" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G447" s="6"/>
     </row>
-    <row r="448" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="448" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G448" s="6"/>
     </row>
-    <row r="449" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="449" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G449" s="6"/>
     </row>
-    <row r="450" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="450" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G450" s="6"/>
     </row>
-    <row r="451" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="451" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G451" s="6"/>
     </row>
-    <row r="452" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="452" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G452" s="6"/>
     </row>
-    <row r="453" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="453" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G453" s="6"/>
     </row>
-    <row r="454" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="454" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G454" s="6"/>
     </row>
-    <row r="455" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="455" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G455" s="6"/>
     </row>
-    <row r="456" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="456" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G456" s="6"/>
     </row>
-    <row r="457" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="457" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G457" s="6"/>
     </row>
-    <row r="458" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="458" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G458" s="6"/>
     </row>
-    <row r="459" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="459" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G459" s="6"/>
     </row>
-    <row r="460" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="460" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G460" s="6"/>
     </row>
-    <row r="461" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="461" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G461" s="6"/>
     </row>
-    <row r="462" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="462" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G462" s="6"/>
     </row>
-    <row r="463" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="463" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G463" s="6"/>
     </row>
-    <row r="464" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="464" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G464" s="6"/>
     </row>
-    <row r="465" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="465" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G465" s="6"/>
     </row>
-    <row r="466" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="466" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G466" s="6"/>
     </row>
-    <row r="467" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="467" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G467" s="6"/>
     </row>
-    <row r="468" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="468" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G468" s="6"/>
     </row>
-    <row r="469" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="469" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G469" s="6"/>
     </row>
-    <row r="470" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="470" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G470" s="6"/>
     </row>
-    <row r="471" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="471" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G471" s="6"/>
     </row>
-    <row r="472" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="472" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G472" s="6"/>
     </row>
-    <row r="473" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="473" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G473" s="6"/>
     </row>
-    <row r="474" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="474" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G474" s="6"/>
     </row>
-    <row r="475" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="475" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G475" s="6"/>
     </row>
-    <row r="476" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="476" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G476" s="6"/>
     </row>
-    <row r="477" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="477" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G477" s="6"/>
     </row>
-    <row r="478" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="478" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G478" s="6"/>
     </row>
-    <row r="479" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="479" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G479" s="6"/>
     </row>
-    <row r="480" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="480" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G480" s="6"/>
     </row>
-    <row r="481" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="481" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G481" s="6"/>
     </row>
-    <row r="482" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="482" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G482" s="6"/>
     </row>
-    <row r="483" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="483" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G483" s="6"/>
     </row>
-    <row r="484" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="484" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G484" s="6"/>
     </row>
-    <row r="485" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="485" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G485" s="6"/>
     </row>
-    <row r="486" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="486" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G486" s="6"/>
     </row>
-    <row r="487" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="487" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G487" s="6"/>
     </row>
-    <row r="488" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="488" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G488" s="6"/>
     </row>
-    <row r="489" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="489" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G489" s="6"/>
     </row>
-    <row r="490" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="490" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G490" s="6"/>
     </row>
-    <row r="491" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="491" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G491" s="6"/>
     </row>
-    <row r="492" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="492" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G492" s="6"/>
     </row>
-    <row r="493" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="493" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G493" s="6"/>
     </row>
-    <row r="494" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="494" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G494" s="6"/>
     </row>
-    <row r="495" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="495" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G495" s="6"/>
     </row>
-    <row r="496" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="496" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G496" s="6"/>
     </row>
-    <row r="497" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="497" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G497" s="6"/>
     </row>
-    <row r="498" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="498" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G498" s="6"/>
     </row>
-    <row r="499" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="499" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G499" s="6"/>
     </row>
-    <row r="500" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="500" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G500" s="6"/>
       <c r="I500" s="6"/>
     </row>
-    <row r="501" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="501" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I501" s="6"/>
     </row>
-    <row r="502" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="502" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I502" s="6"/>
     </row>
-    <row r="503" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="503" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I503" s="6"/>
     </row>
-    <row r="504" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="504" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I504" s="6"/>
     </row>
-    <row r="505" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="505" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I505" s="6"/>
     </row>
-    <row r="506" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="506" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I506" s="6"/>
     </row>
-    <row r="507" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="507" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I507" s="6"/>
     </row>
-    <row r="508" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="508" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I508" s="6"/>
     </row>
-    <row r="509" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="509" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I509" s="6"/>
     </row>
-    <row r="510" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="510" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I510" s="6"/>
     </row>
-    <row r="511" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="511" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I511" s="6"/>
     </row>
-    <row r="512" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="512" spans="7:9" x14ac:dyDescent="0.2">
       <c r="I512" s="6"/>
     </row>
-    <row r="513" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="513" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I513" s="6"/>
     </row>
-    <row r="514" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="514" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I514" s="6"/>
     </row>
-    <row r="515" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="515" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I515" s="6"/>
     </row>
-    <row r="516" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="516" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I516" s="6"/>
     </row>
-    <row r="517" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="517" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I517" s="6"/>
     </row>
-    <row r="518" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="518" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I518" s="6"/>
     </row>
-    <row r="519" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="519" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I519" s="6"/>
     </row>
-    <row r="520" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="520" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I520" s="6"/>
     </row>
-    <row r="521" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="521" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I521" s="6"/>
     </row>
-    <row r="522" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="522" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I522" s="6"/>
     </row>
-    <row r="523" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="523" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I523" s="6"/>
     </row>
-    <row r="524" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="524" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I524" s="6"/>
     </row>
-    <row r="525" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="525" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I525" s="6"/>
     </row>
-    <row r="526" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="526" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I526" s="6"/>
     </row>
-    <row r="527" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="527" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I527" s="6"/>
     </row>
-    <row r="528" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="528" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I528" s="6"/>
     </row>
-    <row r="529" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="529" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I529" s="6"/>
     </row>
-    <row r="530" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="530" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I530" s="6"/>
     </row>
-    <row r="531" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="531" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I531" s="6"/>
     </row>
-    <row r="532" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="532" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I532" s="6"/>
     </row>
-    <row r="533" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="533" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I533" s="6"/>
     </row>
-    <row r="534" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="534" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I534" s="6"/>
     </row>
-    <row r="535" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="535" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I535" s="6"/>
     </row>
-    <row r="536" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="536" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I536" s="6"/>
     </row>
-    <row r="537" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="537" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I537" s="6"/>
     </row>
-    <row r="538" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="538" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I538" s="6"/>
     </row>
-    <row r="539" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="539" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I539" s="6"/>
     </row>
-    <row r="540" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="540" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I540" s="6"/>
     </row>
-    <row r="541" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="541" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I541" s="6"/>
     </row>
-    <row r="542" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="542" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I542" s="6"/>
     </row>
-    <row r="543" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="543" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I543" s="6"/>
     </row>
-    <row r="544" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="544" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I544" s="6"/>
     </row>
-    <row r="545" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="545" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I545" s="6"/>
     </row>
-    <row r="546" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="546" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I546" s="6"/>
     </row>
-    <row r="547" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="547" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I547" s="6"/>
     </row>
-    <row r="548" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="548" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I548" s="6"/>
     </row>
-    <row r="549" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="549" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I549" s="6"/>
     </row>
-    <row r="550" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="550" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I550" s="6"/>
     </row>
-    <row r="551" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="551" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I551" s="6"/>
     </row>
-    <row r="552" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="552" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I552" s="6"/>
     </row>
-    <row r="553" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="553" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I553" s="6"/>
     </row>
-    <row r="554" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="554" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I554" s="6"/>
     </row>
-    <row r="555" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="555" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I555" s="6"/>
     </row>
-    <row r="556" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="556" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I556" s="6"/>
     </row>
-    <row r="557" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="557" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I557" s="6"/>
     </row>
-    <row r="558" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="558" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I558" s="6"/>
     </row>
-    <row r="559" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="559" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I559" s="6"/>
     </row>
-    <row r="560" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="560" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I560" s="6"/>
     </row>
-    <row r="561" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="561" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I561" s="6"/>
     </row>
-    <row r="562" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="562" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I562" s="6"/>
     </row>
-    <row r="563" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="563" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I563" s="6"/>
     </row>
-    <row r="564" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="564" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I564" s="6"/>
     </row>
-    <row r="565" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="565" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I565" s="6"/>
     </row>
-    <row r="566" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="566" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I566" s="6"/>
     </row>
-    <row r="567" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="567" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I567" s="6"/>
     </row>
-    <row r="568" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="568" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I568" s="6"/>
     </row>
-    <row r="569" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="569" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I569" s="6"/>
     </row>
-    <row r="570" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="570" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I570" s="6"/>
     </row>
-    <row r="571" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="571" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I571" s="6"/>
     </row>
-    <row r="572" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="572" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I572" s="6"/>
     </row>
-    <row r="573" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="573" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I573" s="6"/>
     </row>
-    <row r="574" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="574" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I574" s="6"/>
     </row>
-    <row r="575" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="575" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I575" s="6"/>
     </row>
-    <row r="576" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="576" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I576" s="6"/>
     </row>
-    <row r="577" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="577" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I577" s="6"/>
     </row>
-    <row r="578" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="578" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I578" s="6"/>
     </row>
-    <row r="579" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="579" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I579" s="6"/>
     </row>
-    <row r="580" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="580" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I580" s="6"/>
     </row>
-    <row r="581" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="581" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I581" s="6"/>
     </row>
-    <row r="582" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="582" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I582" s="6"/>
     </row>
-    <row r="583" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="583" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I583" s="6"/>
     </row>
-    <row r="584" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="584" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I584" s="6"/>
     </row>
-    <row r="585" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="585" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I585" s="6"/>
     </row>
-    <row r="586" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="586" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I586" s="6"/>
     </row>
-    <row r="587" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="587" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I587" s="6"/>
     </row>
-    <row r="588" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="588" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I588" s="6"/>
     </row>
-    <row r="589" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="589" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I589" s="6"/>
     </row>
-    <row r="590" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="590" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I590" s="6"/>
     </row>
-    <row r="591" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="591" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I591" s="6"/>
     </row>
-    <row r="592" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="592" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I592" s="6"/>
     </row>
-    <row r="593" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="593" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I593" s="6"/>
     </row>
-    <row r="594" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="594" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I594" s="6"/>
     </row>
-    <row r="595" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="595" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I595" s="6"/>
     </row>
-    <row r="596" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="596" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I596" s="6"/>
     </row>
-    <row r="597" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="597" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I597" s="6"/>
     </row>
-    <row r="598" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="598" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I598" s="6"/>
     </row>
-    <row r="599" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="599" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I599" s="6"/>
     </row>
-    <row r="600" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="600" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I600" s="6"/>
     </row>
-    <row r="601" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="601" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I601" s="6"/>
     </row>
-    <row r="602" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="602" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I602" s="6"/>
     </row>
-    <row r="603" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="603" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I603" s="6"/>
     </row>
-    <row r="604" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="604" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I604" s="6"/>
     </row>
-    <row r="605" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="605" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I605" s="6"/>
     </row>
-    <row r="606" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="606" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I606" s="6"/>
     </row>
-    <row r="607" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="607" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I607" s="6"/>
     </row>
-    <row r="608" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="608" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I608" s="6"/>
     </row>
-    <row r="609" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="609" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I609" s="6"/>
     </row>
-    <row r="610" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="610" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I610" s="6"/>
     </row>
-    <row r="611" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="611" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I611" s="6"/>
     </row>
-    <row r="612" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="612" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I612" s="6"/>
     </row>
-    <row r="613" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="613" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I613" s="6"/>
     </row>
-    <row r="614" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="614" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I614" s="6"/>
     </row>
-    <row r="615" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="615" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I615" s="6"/>
     </row>
-    <row r="616" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="616" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I616" s="6"/>
     </row>
-    <row r="617" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="617" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I617" s="6"/>
     </row>
-    <row r="618" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="618" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I618" s="6"/>
     </row>
-    <row r="619" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="619" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I619" s="6"/>
     </row>
-    <row r="620" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="620" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I620" s="6"/>
     </row>
-    <row r="621" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="621" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I621" s="6"/>
     </row>
-    <row r="622" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="622" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I622" s="6"/>
     </row>
-    <row r="623" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="623" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I623" s="6"/>
     </row>
-    <row r="624" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="624" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I624" s="6"/>
     </row>
-    <row r="625" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="625" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I625" s="6"/>
     </row>
-    <row r="626" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="626" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I626" s="6"/>
     </row>
-    <row r="627" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="627" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I627" s="6"/>
     </row>
-    <row r="628" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="628" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I628" s="6"/>
     </row>
-    <row r="629" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="629" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I629" s="6"/>
     </row>
-    <row r="630" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="630" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I630" s="6"/>
     </row>
-    <row r="631" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="631" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I631" s="6"/>
     </row>
-    <row r="632" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="632" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I632" s="6"/>
     </row>
-    <row r="633" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="633" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I633" s="6"/>
     </row>
-    <row r="634" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="634" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I634" s="6"/>
     </row>
-    <row r="635" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="635" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I635" s="6"/>
     </row>
-    <row r="636" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="636" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I636" s="6"/>
     </row>
-    <row r="637" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="637" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I637" s="6"/>
     </row>
-    <row r="638" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="638" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I638" s="6"/>
     </row>
-    <row r="639" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="639" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I639" s="6"/>
     </row>
-    <row r="640" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="640" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I640" s="6"/>
     </row>
-    <row r="641" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="641" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I641" s="6"/>
     </row>
-    <row r="642" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="642" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I642" s="6"/>
     </row>
-    <row r="643" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="643" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I643" s="6"/>
     </row>
-    <row r="644" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="644" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I644" s="6"/>
     </row>
-    <row r="645" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="645" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I645" s="6"/>
     </row>
-    <row r="646" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="646" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I646" s="6"/>
     </row>
-    <row r="647" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="647" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I647" s="6"/>
     </row>
-    <row r="648" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="648" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I648" s="6"/>
     </row>
-    <row r="649" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="649" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I649" s="6"/>
     </row>
-    <row r="650" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="650" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I650" s="6"/>
     </row>
-    <row r="651" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="651" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I651" s="6"/>
     </row>
-    <row r="652" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="652" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I652" s="6"/>
     </row>
-    <row r="653" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="653" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I653" s="6"/>
     </row>
-    <row r="654" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="654" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I654" s="6"/>
     </row>
-    <row r="655" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="655" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I655" s="6"/>
     </row>
-    <row r="656" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="656" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I656" s="6"/>
     </row>
-    <row r="657" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="657" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I657" s="6"/>
     </row>
-    <row r="658" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="658" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I658" s="6"/>
     </row>
-    <row r="659" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="659" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I659" s="6"/>
     </row>
-    <row r="660" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="660" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I660" s="6"/>
     </row>
-    <row r="661" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="661" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I661" s="6"/>
     </row>
-    <row r="662" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="662" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I662" s="6"/>
     </row>
-    <row r="663" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="663" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I663" s="6"/>
     </row>
-    <row r="664" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="664" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I664" s="6"/>
     </row>
-    <row r="665" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="665" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I665" s="6"/>
     </row>
-    <row r="666" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="666" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I666" s="6"/>
     </row>
-    <row r="667" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="667" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I667" s="6"/>
     </row>
-    <row r="668" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="668" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I668" s="6"/>
     </row>
-    <row r="669" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="669" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I669" s="6"/>
     </row>
-    <row r="670" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="670" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I670" s="6"/>
     </row>
-    <row r="671" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="671" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I671" s="6"/>
     </row>
-    <row r="672" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="672" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I672" s="6"/>
     </row>
-    <row r="673" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="673" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I673" s="6"/>
     </row>
-    <row r="674" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="674" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I674" s="6"/>
     </row>
-    <row r="675" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="675" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I675" s="6"/>
     </row>
-    <row r="676" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="676" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I676" s="6"/>
     </row>
-    <row r="677" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="677" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I677" s="6"/>
     </row>
-    <row r="678" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="678" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I678" s="6"/>
     </row>
-    <row r="679" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="679" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I679" s="6"/>
     </row>
-    <row r="680" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="680" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I680" s="6"/>
     </row>
-    <row r="681" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="681" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I681" s="6"/>
     </row>
-    <row r="682" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="682" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I682" s="6"/>
     </row>
-    <row r="683" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="683" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I683" s="6"/>
     </row>
-    <row r="684" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="684" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I684" s="6"/>
     </row>
-    <row r="685" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="685" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I685" s="6"/>
     </row>
-    <row r="686" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="686" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I686" s="6"/>
     </row>
-    <row r="687" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="687" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I687" s="6"/>
     </row>
-    <row r="688" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="688" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I688" s="6"/>
     </row>
-    <row r="689" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="689" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I689" s="6"/>
     </row>
-    <row r="690" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="690" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I690" s="6"/>
     </row>
-    <row r="691" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="691" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I691" s="6"/>
     </row>
-    <row r="692" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="692" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I692" s="6"/>
     </row>
-    <row r="693" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="693" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I693" s="6"/>
     </row>
-    <row r="694" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="694" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I694" s="6"/>
     </row>
-    <row r="695" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="695" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I695" s="6"/>
     </row>
-    <row r="696" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="696" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I696" s="6"/>
     </row>
-    <row r="697" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="697" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I697" s="6"/>
     </row>
-    <row r="698" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="698" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I698" s="6"/>
     </row>
-    <row r="699" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="699" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I699" s="6"/>
     </row>
-    <row r="700" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="700" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I700" s="6"/>
     </row>
-    <row r="701" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="701" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I701" s="6"/>
     </row>
-    <row r="702" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="702" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I702" s="6"/>
     </row>
-    <row r="703" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="703" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I703" s="6"/>
     </row>
-    <row r="704" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="704" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I704" s="6"/>
     </row>
-    <row r="705" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="705" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I705" s="6"/>
     </row>
-    <row r="706" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="706" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I706" s="6"/>
     </row>
-    <row r="707" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="707" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I707" s="6"/>
     </row>
-    <row r="708" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="708" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I708" s="6"/>
     </row>
-    <row r="709" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="709" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I709" s="6"/>
     </row>
-    <row r="710" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="710" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I710" s="6"/>
     </row>
-    <row r="711" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="711" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I711" s="6"/>
     </row>
-    <row r="712" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="712" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I712" s="6"/>
     </row>
-    <row r="713" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="713" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I713" s="6"/>
     </row>
-    <row r="714" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="714" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I714" s="6"/>
     </row>
-    <row r="715" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="715" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I715" s="6"/>
     </row>
-    <row r="716" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="716" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I716" s="6"/>
     </row>
-    <row r="717" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="717" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I717" s="6"/>
     </row>
-    <row r="718" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="718" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I718" s="6"/>
     </row>
-    <row r="719" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="719" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I719" s="6"/>
     </row>
-    <row r="720" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="720" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I720" s="6"/>
     </row>
-    <row r="721" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="721" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I721" s="6"/>
     </row>
-    <row r="722" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="722" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I722" s="6"/>
     </row>
-    <row r="723" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="723" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I723" s="6"/>
     </row>
-    <row r="724" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="724" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I724" s="6"/>
     </row>
-    <row r="725" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="725" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I725" s="6"/>
     </row>
-    <row r="726" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="726" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I726" s="6"/>
     </row>
-    <row r="727" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="727" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I727" s="6"/>
     </row>
-    <row r="728" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="728" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I728" s="6"/>
     </row>
-    <row r="729" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="729" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I729" s="6"/>
     </row>
-    <row r="730" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="730" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I730" s="6"/>
     </row>
-    <row r="731" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="731" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I731" s="6"/>
     </row>
-    <row r="732" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="732" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I732" s="6"/>
     </row>
-    <row r="733" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="733" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I733" s="6"/>
     </row>
-    <row r="734" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="734" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I734" s="6"/>
     </row>
-    <row r="735" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="735" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I735" s="6"/>
     </row>
-    <row r="736" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="736" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I736" s="6"/>
     </row>
-    <row r="737" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="737" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I737" s="6"/>
     </row>
-    <row r="738" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="738" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I738" s="6"/>
     </row>
-    <row r="739" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="739" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I739" s="6"/>
     </row>
-    <row r="740" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="740" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I740" s="6"/>
     </row>
-    <row r="741" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="741" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I741" s="6"/>
     </row>
-    <row r="742" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="742" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I742" s="6"/>
     </row>
-    <row r="743" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="743" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I743" s="6"/>
     </row>
-    <row r="744" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="744" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I744" s="6"/>
     </row>
-    <row r="745" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="745" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I745" s="6"/>
     </row>
-    <row r="746" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="746" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I746" s="6"/>
     </row>
-    <row r="747" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="747" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I747" s="6"/>
     </row>
-    <row r="748" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="748" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I748" s="6"/>
     </row>
-    <row r="749" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="749" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I749" s="6"/>
     </row>
-    <row r="750" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="750" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I750" s="6"/>
     </row>
-    <row r="751" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="751" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I751" s="6"/>
     </row>
-    <row r="752" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="752" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I752" s="6"/>
     </row>
-    <row r="753" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="753" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I753" s="6"/>
     </row>
-    <row r="754" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="754" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I754" s="6"/>
     </row>
-    <row r="755" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="755" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I755" s="6"/>
     </row>
-    <row r="756" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="756" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I756" s="6"/>
     </row>
-    <row r="757" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="757" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I757" s="6"/>
     </row>
-    <row r="758" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="758" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I758" s="6"/>
     </row>
-    <row r="759" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="759" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I759" s="6"/>
     </row>
-    <row r="760" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="760" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I760" s="6"/>
     </row>
-    <row r="761" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="761" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I761" s="6"/>
     </row>
-    <row r="762" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="762" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I762" s="6"/>
     </row>
-    <row r="763" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="763" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I763" s="6"/>
     </row>
-    <row r="764" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="764" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I764" s="6"/>
     </row>
-    <row r="765" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="765" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I765" s="6"/>
     </row>
-    <row r="766" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="766" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I766" s="6"/>
     </row>
-    <row r="767" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="767" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I767" s="6"/>
     </row>
-    <row r="768" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="768" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I768" s="6"/>
     </row>
-    <row r="769" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="769" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I769" s="6"/>
     </row>
-    <row r="770" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="770" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I770" s="6"/>
     </row>
-    <row r="771" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="771" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I771" s="6"/>
     </row>
-    <row r="772" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="772" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I772" s="6"/>
     </row>
-    <row r="773" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="773" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I773" s="6"/>
     </row>
-    <row r="774" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="774" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I774" s="6"/>
     </row>
-    <row r="775" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="775" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I775" s="6"/>
     </row>
-    <row r="776" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="776" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I776" s="6"/>
     </row>
-    <row r="777" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="777" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I777" s="6"/>
     </row>
-    <row r="778" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="778" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I778" s="6"/>
     </row>
-    <row r="779" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="779" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I779" s="6"/>
     </row>
-    <row r="780" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="780" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I780" s="6"/>
     </row>
-    <row r="781" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="781" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I781" s="6"/>
     </row>
-    <row r="782" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="782" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I782" s="6"/>
     </row>
-    <row r="783" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="783" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I783" s="6"/>
     </row>
-    <row r="784" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="784" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I784" s="6"/>
     </row>
-    <row r="785" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="785" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I785" s="6"/>
     </row>
-    <row r="786" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="786" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I786" s="6"/>
     </row>
-    <row r="787" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="787" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I787" s="6"/>
     </row>
-    <row r="788" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="788" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I788" s="6"/>
     </row>
-    <row r="789" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="789" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I789" s="6"/>
     </row>
-    <row r="790" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="790" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I790" s="6"/>
     </row>
-    <row r="791" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="791" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I791" s="6"/>
     </row>
-    <row r="792" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="792" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I792" s="6"/>
     </row>
-    <row r="793" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="793" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I793" s="6"/>
     </row>
-    <row r="794" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="794" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I794" s="6"/>
     </row>
-    <row r="795" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="795" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I795" s="6"/>
     </row>
-    <row r="796" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="796" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I796" s="6"/>
     </row>
-    <row r="797" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="797" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I797" s="6"/>
     </row>
-    <row r="798" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="798" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I798" s="6"/>
     </row>
-    <row r="799" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="799" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I799" s="6"/>
     </row>
-    <row r="800" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="800" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I800" s="6"/>
     </row>
-    <row r="801" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="801" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I801" s="6"/>
     </row>
-    <row r="802" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="802" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I802" s="6"/>
     </row>
-    <row r="803" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="803" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I803" s="6"/>
     </row>
-    <row r="804" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="804" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I804" s="6"/>
     </row>
-    <row r="805" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="805" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I805" s="6"/>
     </row>
-    <row r="806" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="806" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I806" s="6"/>
     </row>
-    <row r="807" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="807" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I807" s="6"/>
     </row>
-    <row r="808" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="808" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I808" s="6"/>
     </row>
-    <row r="809" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="809" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I809" s="6"/>
     </row>
-    <row r="810" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="810" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I810" s="6"/>
     </row>
-    <row r="811" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="811" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I811" s="6"/>
     </row>
-    <row r="812" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="812" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I812" s="6"/>
     </row>
-    <row r="813" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="813" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I813" s="6"/>
     </row>
-    <row r="814" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="814" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I814" s="6"/>
     </row>
-    <row r="815" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="815" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I815" s="6"/>
     </row>
-    <row r="816" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="816" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I816" s="6"/>
     </row>
-    <row r="817" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="817" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I817" s="6"/>
     </row>
-    <row r="818" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="818" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I818" s="6"/>
     </row>
-    <row r="819" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="819" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I819" s="6"/>
     </row>
-    <row r="820" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="820" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I820" s="6"/>
     </row>
-    <row r="821" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="821" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I821" s="6"/>
     </row>
-    <row r="822" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="822" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I822" s="6"/>
     </row>
-    <row r="823" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="823" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I823" s="6"/>
     </row>
-    <row r="824" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="824" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I824" s="6"/>
     </row>
-    <row r="825" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="825" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I825" s="6"/>
     </row>
-    <row r="826" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="826" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I826" s="6"/>
     </row>
-    <row r="827" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="827" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I827" s="6"/>
     </row>
-    <row r="828" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="828" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I828" s="6"/>
     </row>
-    <row r="829" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="829" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I829" s="6"/>
     </row>
-    <row r="830" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="830" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I830" s="6"/>
     </row>
-    <row r="831" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="831" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I831" s="6"/>
     </row>
-    <row r="832" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="832" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I832" s="6"/>
     </row>
-    <row r="833" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="833" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I833" s="6"/>
     </row>
-    <row r="834" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="834" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I834" s="6"/>
     </row>
-    <row r="835" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="835" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I835" s="6"/>
     </row>
-    <row r="836" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="836" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I836" s="6"/>
     </row>
-    <row r="837" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="837" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I837" s="6"/>
     </row>
-    <row r="838" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="838" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I838" s="6"/>
     </row>
-    <row r="839" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="839" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I839" s="6"/>
     </row>
-    <row r="840" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="840" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I840" s="6"/>
     </row>
-    <row r="841" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="841" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I841" s="6"/>
     </row>
-    <row r="842" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="842" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I842" s="6"/>
     </row>
-    <row r="843" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="843" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I843" s="6"/>
     </row>
-    <row r="844" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="844" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I844" s="6"/>
     </row>
-    <row r="845" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="845" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I845" s="6"/>
     </row>
-    <row r="846" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="846" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I846" s="6"/>
     </row>
-    <row r="847" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="847" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I847" s="6"/>
     </row>
-    <row r="848" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="848" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I848" s="6"/>
     </row>
-    <row r="849" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="849" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I849" s="6"/>
     </row>
-    <row r="850" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="850" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I850" s="6"/>
     </row>
-    <row r="851" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="851" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I851" s="6"/>
     </row>
-    <row r="852" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="852" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I852" s="6"/>
     </row>
-    <row r="853" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="853" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I853" s="6"/>
     </row>
-    <row r="854" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="854" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I854" s="6"/>
     </row>
-    <row r="855" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="855" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I855" s="6"/>
     </row>
-    <row r="856" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="856" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I856" s="6"/>
     </row>
-    <row r="857" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="857" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I857" s="6"/>
     </row>
-    <row r="858" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="858" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I858" s="6"/>
     </row>
-    <row r="859" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="859" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I859" s="6"/>
     </row>
-    <row r="860" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="860" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I860" s="6"/>
     </row>
-    <row r="861" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="861" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I861" s="6"/>
     </row>
-    <row r="862" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="862" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I862" s="6"/>
     </row>
-    <row r="863" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="863" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I863" s="6"/>
     </row>
-    <row r="864" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="864" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I864" s="6"/>
     </row>
-    <row r="865" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="865" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I865" s="6"/>
     </row>
-    <row r="866" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="866" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I866" s="6"/>
     </row>
-    <row r="867" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="867" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I867" s="6"/>
     </row>
-    <row r="868" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="868" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I868" s="6"/>
     </row>
-    <row r="869" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="869" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I869" s="6"/>
     </row>
-    <row r="870" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="870" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I870" s="6"/>
     </row>
-    <row r="871" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="871" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I871" s="6"/>
     </row>
-    <row r="872" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="872" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I872" s="6"/>
     </row>
-    <row r="873" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="873" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I873" s="6"/>
     </row>
-    <row r="874" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="874" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I874" s="6"/>
     </row>
-    <row r="875" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="875" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I875" s="6"/>
     </row>
-    <row r="876" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="876" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I876" s="6"/>
     </row>
-    <row r="877" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="877" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I877" s="6"/>
     </row>
-    <row r="878" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="878" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I878" s="6"/>
     </row>
-    <row r="879" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="879" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I879" s="6"/>
     </row>
-    <row r="880" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="880" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I880" s="6"/>
     </row>
-    <row r="881" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="881" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I881" s="6"/>
     </row>
-    <row r="882" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="882" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I882" s="6"/>
     </row>
-    <row r="883" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="883" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I883" s="6"/>
     </row>
-    <row r="884" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="884" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I884" s="6"/>
     </row>
-    <row r="885" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="885" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I885" s="6"/>
     </row>
-    <row r="886" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="886" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I886" s="6"/>
     </row>
-    <row r="887" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="887" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I887" s="6"/>
     </row>
-    <row r="888" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="888" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I888" s="6"/>
     </row>
-    <row r="889" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="889" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I889" s="6"/>
     </row>
-    <row r="890" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="890" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I890" s="6"/>
     </row>
-    <row r="891" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="891" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I891" s="6"/>
     </row>
-    <row r="892" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="892" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I892" s="6"/>
     </row>
-    <row r="893" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="893" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I893" s="6"/>
     </row>
-    <row r="894" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="894" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I894" s="6"/>
     </row>
-    <row r="895" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="895" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I895" s="6"/>
     </row>
-    <row r="896" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="896" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I896" s="6"/>
     </row>
-    <row r="897" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="897" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I897" s="6"/>
     </row>
-    <row r="898" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="898" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I898" s="6"/>
     </row>
-    <row r="899" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="899" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I899" s="6"/>
     </row>
-    <row r="900" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="900" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I900" s="6"/>
     </row>
-    <row r="901" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="901" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I901" s="6"/>
     </row>
-    <row r="902" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="902" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I902" s="6"/>
     </row>
-    <row r="903" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="903" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I903" s="6"/>
     </row>
-    <row r="904" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="904" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I904" s="6"/>
     </row>
-    <row r="905" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="905" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I905" s="6"/>
     </row>
-    <row r="906" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="906" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I906" s="6"/>
     </row>
-    <row r="907" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="907" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I907" s="6"/>
     </row>
-    <row r="908" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="908" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I908" s="6"/>
     </row>
-    <row r="909" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="909" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I909" s="6"/>
     </row>
-    <row r="910" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="910" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I910" s="6"/>
     </row>
-    <row r="911" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="911" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I911" s="6"/>
     </row>
-    <row r="912" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="912" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I912" s="6"/>
     </row>
-    <row r="913" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="913" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I913" s="6"/>
     </row>
-    <row r="914" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="914" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I914" s="6"/>
     </row>
-    <row r="915" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="915" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I915" s="6"/>
     </row>
-    <row r="916" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="916" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I916" s="6"/>
     </row>
-    <row r="917" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="917" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I917" s="6"/>
     </row>
-    <row r="918" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="918" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I918" s="6"/>
     </row>
-    <row r="919" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="919" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I919" s="6"/>
     </row>
-    <row r="920" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="920" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I920" s="6"/>
     </row>
-    <row r="921" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="921" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I921" s="6"/>
     </row>
-    <row r="922" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="922" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I922" s="6"/>
     </row>
-    <row r="923" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="923" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I923" s="6"/>
     </row>
-    <row r="924" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="924" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I924" s="6"/>
     </row>
-    <row r="925" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="925" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I925" s="6"/>
     </row>
-    <row r="926" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="926" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I926" s="6"/>
     </row>
-    <row r="927" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="927" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I927" s="6"/>
     </row>
-    <row r="928" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="928" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I928" s="6"/>
     </row>
-    <row r="929" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="929" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I929" s="6"/>
     </row>
-    <row r="930" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="930" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I930" s="6"/>
     </row>
-    <row r="931" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="931" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I931" s="6"/>
     </row>
-    <row r="932" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="932" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I932" s="6"/>
     </row>
-    <row r="933" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="933" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I933" s="6"/>
     </row>
-    <row r="934" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="934" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I934" s="6"/>
     </row>
-    <row r="935" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="935" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I935" s="6"/>
     </row>
-    <row r="936" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="936" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I936" s="6"/>
     </row>
-    <row r="937" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="937" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I937" s="6"/>
     </row>
-    <row r="938" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="938" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I938" s="6"/>
     </row>
-    <row r="939" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="939" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I939" s="6"/>
     </row>
-    <row r="940" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="940" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I940" s="6"/>
     </row>
-    <row r="941" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="941" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I941" s="6"/>
     </row>
-    <row r="942" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="942" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I942" s="6"/>
     </row>
-    <row r="943" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="943" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I943" s="6"/>
     </row>
-    <row r="944" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="944" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I944" s="6"/>
     </row>
-    <row r="945" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="945" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I945" s="6"/>
     </row>
-    <row r="946" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="946" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I946" s="6"/>
     </row>
-    <row r="947" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="947" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I947" s="6"/>
     </row>
-    <row r="948" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="948" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I948" s="6"/>
     </row>
-    <row r="949" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="949" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I949" s="6"/>
     </row>
-    <row r="950" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="950" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I950" s="6"/>
     </row>
-    <row r="951" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="951" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I951" s="6"/>
     </row>
-    <row r="952" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="952" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I952" s="6"/>
     </row>
-    <row r="953" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="953" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I953" s="6"/>
     </row>
-    <row r="954" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="954" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I954" s="6"/>
     </row>
-    <row r="955" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="955" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I955" s="6"/>
     </row>
-    <row r="956" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="956" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I956" s="6"/>
     </row>
-    <row r="957" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="957" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I957" s="6"/>
     </row>
-    <row r="958" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="958" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I958" s="6"/>
     </row>
-    <row r="959" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="959" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I959" s="6"/>
     </row>
-    <row r="960" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="960" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I960" s="6"/>
     </row>
-    <row r="961" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="961" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I961" s="6"/>
     </row>
-    <row r="962" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="962" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I962" s="6"/>
     </row>
-    <row r="963" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="963" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I963" s="6"/>
     </row>
-    <row r="964" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="964" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I964" s="6"/>
     </row>
-    <row r="965" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="965" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I965" s="6"/>
     </row>
-    <row r="966" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="966" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I966" s="6"/>
     </row>
-    <row r="967" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="967" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I967" s="6"/>
     </row>
-    <row r="968" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="968" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I968" s="6"/>
     </row>
-    <row r="969" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="969" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I969" s="6"/>
     </row>
-    <row r="970" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="970" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I970" s="6"/>
     </row>
-    <row r="971" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="971" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I971" s="6"/>
     </row>
-    <row r="972" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="972" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I972" s="6"/>
     </row>
-    <row r="973" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="973" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I973" s="6"/>
     </row>
-    <row r="974" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="974" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I974" s="6"/>
     </row>
-    <row r="975" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="975" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I975" s="6"/>
     </row>
-    <row r="976" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="976" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I976" s="6"/>
     </row>
-    <row r="977" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="977" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I977" s="6"/>
     </row>
-    <row r="978" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="978" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I978" s="6"/>
     </row>
-    <row r="979" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="979" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I979" s="6"/>
     </row>
-    <row r="980" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="980" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I980" s="6"/>
     </row>
-    <row r="981" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="981" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I981" s="6"/>
     </row>
-    <row r="982" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="982" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I982" s="6"/>
     </row>
-    <row r="983" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="983" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I983" s="6"/>
     </row>
-    <row r="984" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="984" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I984" s="6"/>
     </row>
-    <row r="985" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="985" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I985" s="6"/>
     </row>
-    <row r="986" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="986" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I986" s="6"/>
     </row>
-    <row r="987" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="987" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I987" s="6"/>
     </row>
-    <row r="988" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="988" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I988" s="6"/>
     </row>
-    <row r="989" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="989" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I989" s="6"/>
     </row>
-    <row r="990" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="990" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I990" s="6"/>
     </row>
-    <row r="991" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="991" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I991" s="6"/>
     </row>
-    <row r="992" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="992" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I992" s="6"/>
     </row>
-    <row r="993" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="993" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I993" s="6"/>
     </row>
-    <row r="994" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="994" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I994" s="6"/>
     </row>
-    <row r="995" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="995" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I995" s="6"/>
     </row>
-    <row r="996" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="996" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I996" s="6"/>
     </row>
-    <row r="997" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="997" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I997" s="6"/>
     </row>
-    <row r="998" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="998" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I998" s="6"/>
     </row>
-    <row r="999" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="999" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I999" s="6"/>
     </row>
-    <row r="1000" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="1000" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I1000" s="6"/>
     </row>
   </sheetData>
@@ -3700,19 +3700,19 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3730,16 +3730,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>